<commit_message>
add examples of usecols and skiprows
</commit_message>
<xml_diff>
--- a/pandas-excel/example.xlsx
+++ b/pandas-excel/example.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="1" r:id="rId1"/>
     <sheet name="header" sheetId="2" r:id="rId2"/>
     <sheet name="dualheader" sheetId="3" r:id="rId3"/>
     <sheet name="colheader" sheetId="4" r:id="rId4"/>
+    <sheet name="skiprow" sheetId="5" r:id="rId5"/>
+    <sheet name="usecols" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,6 +110,30 @@
   </si>
   <si>
     <t>address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seoul</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pusan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>population</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -695,4 +721,139 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>5000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>